<commit_message>
updates to remove dummy imports; high RE stress test; scenario to reduce model size by eliminating solar/wind slices that did not penetrate.
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_BaseEXTRA.xlsx
+++ b/SuppXLS/Scen_BaseEXTRA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IEMM\IEMM_MIG\IEMM_V60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9480DFE-3120-4301-942A-BE5884790649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2F2202-E0CA-4E8B-A944-5065758BB4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8370" yWindow="3510" windowWidth="16740" windowHeight="11385" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="17" r:id="rId1"/>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11366" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11369" uniqueCount="166">
   <si>
     <t>Year</t>
   </si>
@@ -729,6 +729,9 @@
   <si>
     <t>Demht*,-*in</t>
   </si>
+  <si>
+    <t>*WOF*,-*tran_near*,-*shal_near*</t>
+  </si>
 </sst>
 </file>
 
@@ -925,7 +928,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
@@ -943,6 +946,7 @@
     <xf numFmtId="2" fontId="11" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1482,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:W92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -72770,8 +72774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:P21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72922,6 +72926,20 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14">
+        <v>2100</v>
+      </c>
+    </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>72</v>

</xml_diff>